<commit_message>
Migrate baseline and formula fixtures to shared corpus
Co-authored-by: Shri Sukhani <shrisukhani@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/apps/spreadsheet-core-rs/fixtures/compat_baseline.xlsx
+++ b/apps/spreadsheet-core-rs/fixtures/compat_baseline.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Region</t>
   </si>
@@ -26,13 +26,16 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Active</t>
+  </si>
+  <si>
     <t>North</t>
   </si>
   <si>
     <t>South</t>
   </si>
   <si>
-    <t>Generated fixture workbook</t>
+    <t>Generated from fixture workbook</t>
   </si>
 </sst>
 </file>
@@ -364,13 +367,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,10 +383,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>120</v>
@@ -392,10 +398,13 @@
         <f>SUM(B2:B3)</f>
         <v>200</v>
       </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>80</v>
@@ -416,7 +425,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>